<commit_message>
added 1 test case on register
</commit_message>
<xml_diff>
--- a/test_case_and_bug_report/swagger-note-api-test-case.xlsx
+++ b/test_case_and_bug_report/swagger-note-api-test-case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GitHub\Swagger Note API (Postman)\test_case_and_bug_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6A63A8-4025-4B94-A866-6897ADF9CD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8237D9-F80C-43C4-8E4A-8D9AC3D53BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Swagger Note API" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Swagger Note API'!$B$6:$N$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Swagger Note API'!$B$6:$N$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="448">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -289,60 +289,6 @@
     "name": "{{$randomFullName}}",
     "email": "{{$randomEmail}}",
     "password": "12"
-}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "name": "{{$randomFullName}}",
-    "email": "{{$randomEmail}}",
-    "password": "This is password above thirty characters"
-}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "name": "",
-    "email": "{{email}}",
-    "password": "{{password}}"
 }</t>
     </r>
   </si>
@@ -383,33 +329,6 @@
     <t>This test case simulates a negative scenario in which a user attempts to register an account without providing a password which is mandatory.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "name": "{{$randomFullName}}",
-    "email": "{{email}}",
-    "password": ""
-}</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">This test case simulates a negative scenario in which a user attempts to register an account with all mandatory fields left empty. </t>
   </si>
   <si>
@@ -446,89 +365,10 @@
     <t>This test case simulates a negative scenario in which a user attempts to register an account using a password that falls within the acceptable length range but is considered weak.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "name": "{{$randomFullName}}",
-    "email": "{{$randomEmail}}",
-    "password": "123456"
-}</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">This test case simulates a negative scenario in which a user attempts to register an account using an email address that is already associated with an existing account. </t>
   </si>
   <si>
     <t xml:space="preserve">This test case simulates a negative scenario in which a user attempts to log in without providing an email address in the required field. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "email": "",
-    "password": "123456"
-}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "email": "{{email}}",
-    "password": ""
-}</t>
-    </r>
   </si>
   <si>
     <r>
@@ -595,50 +435,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "email": "{{email}}",
-    "password": "{{$randomPassword}}"
-}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Request Body:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>{
-    "email": "{{email}}",
-    "password": "{{password}}"
-}</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">This test case simulates a positive scenario in which a user attempts to log in using correct email and password. </t>
   </si>
   <si>
@@ -659,74 +455,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>{
-    "name": "{{$randomFullName}}",
-    "email": "{{$randomEmail}}",
-    "password": "123456"
-}</t>
-    </r>
-  </si>
-  <si>
     <t>As Expected</t>
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Request Body:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-{
-    "name": "{{$randomFullName}}",
-    "email": "123@@gmail@com",
-    "password": "123456"
-}</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1282,24 +1014,6 @@
   </si>
   <si>
     <t>This test case simulates a positive scenario in which a user attempts to log in using a new password that they have recently set.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Request Body:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>{
-    "email": "{{email}}",
-    "password": "{{newPass}}"
-}</t>
-    </r>
   </si>
   <si>
     <r>
@@ -3142,34 +2856,6 @@
     <t xml:space="preserve">This test case simulates a negative scenario in which a user attempts to register an account using an email address that is in invalid format. </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1&gt; Open Postman and create a new request and set the HTTP method to POST.
-2&gt; Enter the valid register user endpoint URL </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/users/register</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-3&gt; Add payload body in JSON format with invalid emai address format that doesn't exist.
-4&gt; Click Send button to execute the request.
-5&gt; Verify the response status code and message.
-</t>
-    </r>
-  </si>
-  <si>
     <t>(POST)
 Register User with Empty Name Field.</t>
   </si>
@@ -4308,48 +3994,6 @@
         <family val="1"/>
       </rPr>
       <t>{
-    "currentPassword": "123456",
-    "newPassword": "123456"
-}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Request Header:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">"key" : "x-auth-token"
-"Value" : "{{token}}"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Request Body:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>{
     "currentPassword": "{{password}}",
     "newPassword": "Pr@be"
 }</t>
@@ -4591,90 +4235,6 @@
 4&gt; Add payload body in JSON format where the new password meets desired requirements.
 5&gt; Click Send button to execute the request.
 6&gt; Verify the response status code and message.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Request Header:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">"key" : "x-auth-token"
-"Value" : "{{token}}"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Request Body:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>{
-    "currentPassword": "IncorrectCurrentPassword",
-    "newPassword": "{{newPass}}"
-}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Request Header:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">"key" : "x-auth-token"
-"Value" : "{{token}}"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Request Body:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>{
-    "currentPassword": "Qwerty",
-    "newPassword": "{{newPass}}"
-}</t>
     </r>
   </si>
   <si>
@@ -6641,6 +6201,538 @@
   </si>
   <si>
     <t>TC_071</t>
+  </si>
+  <si>
+    <t>(POST)
+Register User with Non-Existing Email Address.</t>
+  </si>
+  <si>
+    <t>This test case simulates a negative scenario in which a user attempts to register an account using an email address that doesn't exist.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1&gt; Open Postman and create a new request and set the HTTP method to POST.
+2&gt; Enter the valid register user endpoint URL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3333FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/users/register</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+3&gt; Add payload body in JSON format with invalid email address format that doesn't exist.
+4&gt; Click Send button to execute the request.
+5&gt; Verify the response status code and message.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1&gt; Open Postman and create a new request and set the HTTP method to POST.
+2&gt; Enter the valid register user endpoint URL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3333FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/users/register</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+3&gt; Add payload body in JSON format with email address that doesn't exist.
+4&gt; Click Send button to execute the request.
+5&gt; Verify the response status code and message.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "name": "{{$randomFullName}}",
+    "email": "{{invalidEmail}}",
+    "password": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>{
+    "name": "{{$randomFullName}}",
+    "email": "{{$randomEmail}}",
+    "password": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "name": "{{$randomFullName}}",
+    "email": "{{$randomEmail}}",
+    "password": "This is p@ssword @bove thirty (30) char@cters"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "name": "{{$randomFullName}}",
+    "email": "123@@zmail@@com",
+    "password": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "name": "",
+    "email": "{{validEmail}}",
+    "password": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "name": "{{$randomFullName}}",
+    "email": "{{validEmail}}",
+    "password": ""
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "name": "{{$randomFullName}}",
+    "email": "{{$randomEmail}}",
+    "password": "{{weakPassword}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "name": "{{$randomFullName}}",
+    "email": "{{validEmail}}",
+    "password": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "email": "",
+    "password": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "email": "{{validEmail}}",
+    "password": ""
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Request Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "email": "{{validEmail}}",
+    "password": "{{$randomPassword}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Request Body:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>{
+    "email": "{{validEmail}}",
+    "password": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Request Header:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">"key" : "x-auth-token"
+"Value" : "{{token}}"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Request Body:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>{
+    "currentPassword": "{{password}}",
+    "newPassword": "{{password}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Request Header:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">"key" : "x-auth-token"
+"Value" : "{{token}}"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Request Body:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>{
+    "currentPassword": "IncorrectCurrentPassword",
+    "newPassword": "{{newPassword}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Request Header:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">"key" : "x-auth-token"
+"Value" : "{{token}}"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Request Body:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>{
+    "currentPassword": "{{weakPassword}}",
+    "newPassword": "{{newPassword}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Request Body:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>{
+    "email": "{{validEmail}}",
+    "password": "{{newPassword}}"
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_072</t>
   </si>
 </sst>
 </file>
@@ -6982,11 +7074,11 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7212,13 +7304,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD1042"/>
+  <dimension ref="A1:AD1043"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H46" sqref="H46"/>
+      <selection pane="bottomRight" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -7228,7 +7320,7 @@
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.5546875" customWidth="1"/>
-    <col min="6" max="6" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="42.44140625" customWidth="1"/>
     <col min="7" max="7" width="40.33203125" customWidth="1"/>
     <col min="8" max="8" width="30.5546875" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
@@ -7240,32 +7332,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
     </row>
     <row r="2" spans="1:30" ht="17.399999999999999">
       <c r="A2" s="3"/>
@@ -7275,7 +7367,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="4" t="s">
@@ -7348,10 +7440,10 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="4" t="s">
@@ -7474,23 +7566,23 @@
         <v>13</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="25" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="18"/>
@@ -7518,25 +7610,25 @@
         <v>16</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>104</v>
+        <v>432</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="18"/>
@@ -7564,25 +7656,25 @@
         <v>18</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>76</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>104</v>
+        <v>432</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="18"/>
@@ -7610,25 +7702,25 @@
         <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>77</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="18"/>
@@ -7656,25 +7748,25 @@
         <v>22</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>78</v>
+        <v>433</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="18"/>
@@ -7702,25 +7794,25 @@
         <v>50</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>263</v>
+        <v>429</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>107</v>
+        <v>434</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="18"/>
@@ -7742,44 +7834,30 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:30" ht="109.2">
+    <row r="13" spans="1:30" ht="148.80000000000001" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>264</v>
+      <c r="C13" s="16" t="s">
+        <v>427</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>80</v>
+        <v>428</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>265</v>
+        <v>430</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>416</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>417</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>415</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="14"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -7796,43 +7874,43 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:30" ht="124.8">
+    <row r="14" spans="1:30" ht="109.2">
       <c r="A14" s="3"/>
       <c r="B14" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>82</v>
+        <v>435</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="M14" s="21" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="N14" s="14"/>
       <c r="O14" s="2"/>
@@ -7850,43 +7928,43 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:30" ht="109.2">
+    <row r="15" spans="1:30" ht="124.8">
       <c r="A15" s="3"/>
       <c r="B15" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>420</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>114</v>
+        <v>403</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="N15" s="14"/>
       <c r="O15" s="2"/>
@@ -7904,43 +7982,43 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:30" ht="124.8">
+    <row r="16" spans="1:30" ht="109.2">
       <c r="A16" s="3"/>
       <c r="B16" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>86</v>
+        <v>436</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J16" s="22" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="N16" s="14"/>
       <c r="O16" s="2"/>
@@ -7958,43 +8036,43 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" ht="220.2" customHeight="1">
+    <row r="17" spans="1:28" ht="124.8">
       <c r="A17" s="3"/>
       <c r="B17" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>440</v>
+        <v>408</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>426</v>
+        <v>407</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="L17" s="18" t="s">
-        <v>12</v>
+        <v>227</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="N17" s="14"/>
       <c r="O17" s="2"/>
@@ -8018,30 +8096,38 @@
         <v>27</v>
       </c>
       <c r="C18" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="F18" s="25" t="s">
         <v>437</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>438</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>439</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>89</v>
-      </c>
       <c r="G18" s="24" t="s">
-        <v>115</v>
+        <v>425</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>105</v>
+        <v>411</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="21"/>
+        <v>104</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>400</v>
+      </c>
       <c r="N18" s="14"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -8058,33 +8144,33 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="124.8">
+    <row r="19" spans="1:28" ht="220.2" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>90</v>
+        <v>423</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>230</v>
+        <v>424</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>89</v>
+        <v>438</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J19" s="21"/>
+        <v>97</v>
+      </c>
+      <c r="J19" s="22"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
       <c r="M19" s="21"/>
@@ -8110,38 +8196,30 @@
         <v>29</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>276</v>
+        <v>219</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>92</v>
+        <v>438</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>425</v>
+        <v>106</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>424</v>
+        <v>96</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J20" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>415</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J20" s="21"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="21"/>
       <c r="N20" s="14"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -8158,43 +8236,43 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="134.25" customHeight="1">
+    <row r="21" spans="1:28" ht="124.8">
       <c r="A21" s="3"/>
       <c r="B21" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>436</v>
+        <v>439</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>410</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="L21" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="N21" s="14"/>
       <c r="O21" s="2"/>
@@ -8212,43 +8290,43 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="124.8">
+    <row r="22" spans="1:28" ht="134.25" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="31" t="s">
-        <v>423</v>
+        <v>440</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>421</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="N22" s="14"/>
       <c r="O22" s="2"/>
@@ -8272,30 +8350,38 @@
         <v>33</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>105</v>
+        <v>88</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>413</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="14"/>
+        <v>104</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="M23" s="21" t="s">
+        <v>400</v>
+      </c>
       <c r="N23" s="14"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -8318,25 +8404,25 @@
         <v>34</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>106</v>
+        <v>96</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="18"/>
@@ -8364,25 +8450,25 @@
         <v>35</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>120</v>
+        <v>441</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J25" s="13"/>
       <c r="K25" s="18"/>
@@ -8404,39 +8490,37 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="234">
+    <row r="26" spans="1:28" ht="124.8">
       <c r="A26" s="3"/>
       <c r="B26" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>287</v>
+      <c r="C26" s="19" t="s">
+        <v>273</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>101</v>
+        <v>274</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>110</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>106</v>
+        <v>96</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="J26" s="13"/>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
       <c r="M26" s="14"/>
-      <c r="N26" s="15" t="s">
-        <v>402</v>
-      </c>
+      <c r="N26" s="14"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -8452,34 +8536,39 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="124.8" customHeight="1">
+    <row r="27" spans="1:28" ht="234">
       <c r="A27" s="3"/>
       <c r="B27" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>291</v>
+        <v>94</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>292</v>
+        <v>276</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>442</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
       <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
+      <c r="N27" s="15" t="s">
+        <v>387</v>
+      </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
@@ -8495,31 +8584,28 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="134.4" customHeight="1">
+    <row r="28" spans="1:28" ht="124.8" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>111</v>
+        <v>280</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>134</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="18"/>
@@ -8541,37 +8627,37 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" ht="187.2">
+    <row r="29" spans="1:28" ht="134.4" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>319</v>
+        <v>277</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>123</v>
+        <v>192</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J29" s="13"/>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
@@ -8587,91 +8673,91 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="185.25" customHeight="1">
+    <row r="30" spans="1:28" ht="187.2">
       <c r="A30" s="3"/>
       <c r="B30" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>406</v>
+        <v>287</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>309</v>
+        <v>192</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>423</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>429</v>
+        <v>113</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J30" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="K30" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="L30" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="M30" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="N30" s="14"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="11"/>
-    </row>
-    <row r="31" spans="1:28" ht="183" customHeight="1">
+        <v>97</v>
+      </c>
+      <c r="J30" s="13"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+    </row>
+    <row r="31" spans="1:28" ht="185.25" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C31" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="F31" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>310</v>
-      </c>
       <c r="G31" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>105</v>
+        <v>408</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>414</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
+        <v>104</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="K31" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="N31" s="14"/>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
@@ -8687,37 +8773,37 @@
       <c r="AA31" s="11"/>
       <c r="AB31" s="11"/>
     </row>
-    <row r="32" spans="1:28" ht="180.75" customHeight="1">
+    <row r="32" spans="1:28" ht="183" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
@@ -8739,25 +8825,25 @@
         <v>44</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J33" s="13"/>
       <c r="K33" s="18"/>
@@ -8779,77 +8865,77 @@
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
     </row>
-    <row r="34" spans="1:28" ht="218.4">
+    <row r="34" spans="1:28" ht="180.75" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="14"/>
       <c r="N34" s="14"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
-    </row>
-    <row r="35" spans="1:28" ht="240" customHeight="1">
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+    </row>
+    <row r="35" spans="1:28" ht="218.4">
       <c r="A35" s="3"/>
       <c r="B35" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>203</v>
+        <v>302</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J35" s="13"/>
       <c r="K35" s="18"/>
@@ -8871,37 +8957,37 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="208.5" customHeight="1">
+    <row r="36" spans="1:28" ht="240" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>333</v>
+        <v>192</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J36" s="13"/>
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="14"/>
-      <c r="N36" s="15"/>
+      <c r="N36" s="14"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
@@ -8917,31 +9003,31 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="193.5" customHeight="1">
+    <row r="37" spans="1:28" ht="208.5" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>103</v>
+        <v>321</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J37" s="13"/>
       <c r="K37" s="18"/>
@@ -8963,45 +9049,37 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="195.75" customHeight="1">
+    <row r="38" spans="1:28" ht="193.5" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>334</v>
+        <v>95</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>239</v>
+        <v>107</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J38" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="K38" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="L38" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="M38" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="N38" s="14"/>
+        <v>97</v>
+      </c>
+      <c r="J38" s="13"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="15"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
@@ -9017,36 +9095,44 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="191.25" customHeight="1">
+    <row r="39" spans="1:28" ht="195.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>105</v>
+        <v>117</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>228</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J39" s="13"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="14"/>
+        <v>104</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M39" s="21" t="s">
+        <v>400</v>
+      </c>
       <c r="N39" s="14"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -9063,36 +9149,36 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="217.5" customHeight="1">
+    <row r="40" spans="1:28" ht="191.25" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>336</v>
+        <v>443</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>105</v>
+        <v>118</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J40" s="21"/>
+        <v>97</v>
+      </c>
+      <c r="J40" s="13"/>
       <c r="K40" s="18"/>
       <c r="L40" s="18"/>
-      <c r="M40" s="21"/>
+      <c r="M40" s="14"/>
       <c r="N40" s="14"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -9109,36 +9195,36 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="193.5" customHeight="1">
+    <row r="41" spans="1:28" ht="217.5" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J41" s="13"/>
+        <v>97</v>
+      </c>
+      <c r="J41" s="21"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
-      <c r="M41" s="14"/>
+      <c r="M41" s="21"/>
       <c r="N41" s="14"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -9155,31 +9241,31 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="201" customHeight="1">
-      <c r="A42" s="1"/>
+    <row r="42" spans="1:28" ht="193.5" customHeight="1">
+      <c r="A42" s="3"/>
       <c r="B42" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J42" s="13"/>
       <c r="K42" s="18"/>
@@ -9201,44 +9287,36 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="200.25" customHeight="1">
+    <row r="43" spans="1:28" ht="201" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="19" t="s">
-        <v>345</v>
+      <c r="C43" s="16" t="s">
+        <v>330</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>431</v>
+        <v>120</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>430</v>
+        <v>96</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J43" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="L43" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="M43" s="21" t="s">
-        <v>415</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="14"/>
       <c r="N43" s="14"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
@@ -9255,37 +9333,45 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="192.75" customHeight="1">
+    <row r="44" spans="1:28" ht="200.25" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>353</v>
+        <v>420</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>105</v>
+        <v>416</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>415</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J44" s="13"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="15"/>
+        <v>104</v>
+      </c>
+      <c r="J44" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="K44" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="L44" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M44" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="N44" s="14"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -9301,37 +9387,37 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="198" customHeight="1">
+    <row r="45" spans="1:28" ht="192.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="16" t="s">
-        <v>354</v>
+      <c r="C45" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>203</v>
+        <v>445</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J45" s="21"/>
+        <v>97</v>
+      </c>
+      <c r="J45" s="13"/>
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
-      <c r="M45" s="21"/>
-      <c r="N45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="15"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -9347,31 +9433,31 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="155.25" customHeight="1">
+    <row r="46" spans="1:28" ht="198" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="13" t="s">
         <v>58</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>105</v>
+        <v>122</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J46" s="21"/>
       <c r="K46" s="18"/>
@@ -9393,31 +9479,31 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="143.25" customHeight="1">
+    <row r="47" spans="1:28" ht="155.25" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="19" t="s">
-        <v>358</v>
+      <c r="C47" s="16" t="s">
+        <v>344</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>133</v>
+        <v>345</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>231</v>
+        <v>342</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J47" s="21"/>
       <c r="K47" s="18"/>
@@ -9439,36 +9525,36 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="234">
+    <row r="48" spans="1:28" ht="143.25" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="16" t="s">
-        <v>361</v>
+      <c r="C48" s="19" t="s">
+        <v>343</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>135</v>
+        <v>442</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="H48" s="13" t="s">
-        <v>105</v>
+        <v>108</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J48" s="13"/>
+        <v>97</v>
+      </c>
+      <c r="J48" s="21"/>
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
-      <c r="M48" s="14"/>
+      <c r="M48" s="21"/>
       <c r="N48" s="14"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
@@ -9485,36 +9571,36 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="124.8">
+    <row r="49" spans="1:28" ht="234">
       <c r="A49" s="1"/>
       <c r="B49" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="26" t="s">
-        <v>362</v>
+      <c r="C49" s="16" t="s">
+        <v>346</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>138</v>
+        <v>446</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="H49" s="16" t="s">
-        <v>105</v>
+        <v>125</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J49" s="21"/>
+        <v>97</v>
+      </c>
+      <c r="J49" s="13"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
-      <c r="M49" s="21"/>
+      <c r="M49" s="14"/>
       <c r="N49" s="14"/>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
@@ -9531,44 +9617,36 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="156">
+    <row r="50" spans="1:28" ht="124.8">
       <c r="A50" s="1"/>
       <c r="B50" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="16" t="s">
-        <v>363</v>
+      <c r="C50" s="26" t="s">
+        <v>347</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>371</v>
+        <v>222</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>423</v>
+        <v>126</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>432</v>
+        <v>96</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J50" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="K50" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="L50" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="M50" s="21" t="s">
-        <v>415</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J50" s="21"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="21"/>
       <c r="N50" s="14"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
@@ -9585,36 +9663,44 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="171.6">
+    <row r="51" spans="1:28" ht="156">
       <c r="A51" s="1"/>
       <c r="B51" s="13" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>105</v>
+        <v>408</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>417</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J51" s="21"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="21"/>
+        <v>104</v>
+      </c>
+      <c r="J51" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="K51" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="L51" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="M51" s="21" t="s">
+        <v>400</v>
+      </c>
       <c r="N51" s="14"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
@@ -9631,31 +9717,31 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="218.4">
+    <row r="52" spans="1:28" ht="156">
       <c r="A52" s="1"/>
       <c r="B52" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J52" s="21"/>
       <c r="K52" s="18"/>
@@ -9677,36 +9763,36 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="171.6">
+    <row r="53" spans="1:28" ht="187.2">
       <c r="A53" s="1"/>
       <c r="B53" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>144</v>
+        <v>350</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J53" s="13"/>
+        <v>97</v>
+      </c>
+      <c r="J53" s="21"/>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
-      <c r="M53" s="14"/>
+      <c r="M53" s="21"/>
       <c r="N53" s="14"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -9723,44 +9809,36 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="296.39999999999998">
+    <row r="54" spans="1:28" ht="156">
       <c r="A54" s="1"/>
       <c r="B54" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>366</v>
+        <v>133</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>372</v>
+        <v>223</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>434</v>
-      </c>
-      <c r="H54" s="16" t="s">
-        <v>433</v>
+        <v>134</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J54" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="K54" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="L54" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="M54" s="21" t="s">
-        <v>415</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J54" s="13"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="14"/>
       <c r="N54" s="14"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -9775,37 +9853,46 @@
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
-    </row>
-    <row r="55" spans="1:28" ht="327.60000000000002">
+      <c r="AB54" s="2"/>
+    </row>
+    <row r="55" spans="1:28" ht="280.8">
       <c r="A55" s="1"/>
       <c r="B55" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="G55" s="25" t="s">
-        <v>149</v>
+        <v>136</v>
+      </c>
+      <c r="G55" s="24" t="s">
+        <v>419</v>
       </c>
       <c r="H55" s="16" t="s">
-        <v>105</v>
+        <v>418</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J55" s="13"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="14"/>
+        <v>104</v>
+      </c>
+      <c r="J55" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="K55" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="L55" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="M55" s="21" t="s">
+        <v>400</v>
+      </c>
       <c r="N55" s="14"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -9820,7 +9907,6 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
-      <c r="AB55" s="2"/>
     </row>
     <row r="56" spans="1:28" ht="327.60000000000002">
       <c r="A56" s="1"/>
@@ -9828,25 +9914,25 @@
         <v>70</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>373</v>
+        <v>392</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="G56" s="24" t="s">
-        <v>150</v>
+        <v>137</v>
+      </c>
+      <c r="G56" s="25" t="s">
+        <v>138</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J56" s="13"/>
       <c r="K56" s="18"/>
@@ -9868,29 +9954,31 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" ht="156">
+    <row r="57" spans="1:28" ht="327.60000000000002">
       <c r="A57" s="1"/>
       <c r="B57" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="F57" s="24"/>
+        <v>358</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>173</v>
+      </c>
       <c r="G57" s="24" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J57" s="13"/>
       <c r="K57" s="18"/>
@@ -9918,25 +10006,23 @@
         <v>72</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>375</v>
+        <v>353</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="F58" s="25" t="s">
-        <v>241</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="F58" s="24"/>
       <c r="G58" s="24" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J58" s="13"/>
       <c r="K58" s="18"/>
@@ -9958,31 +10044,31 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="343.2">
+    <row r="59" spans="1:28" ht="156">
       <c r="A59" s="1"/>
       <c r="B59" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J59" s="13"/>
       <c r="K59" s="18"/>
@@ -10004,31 +10090,31 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" ht="171.6">
+    <row r="60" spans="1:28" ht="343.2">
       <c r="A60" s="1"/>
       <c r="B60" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="F60" s="24" t="s">
-        <v>183</v>
+        <v>366</v>
+      </c>
+      <c r="F60" s="25" t="s">
+        <v>229</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>105</v>
+        <v>149</v>
+      </c>
+      <c r="H60" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J60" s="13"/>
       <c r="K60" s="18"/>
@@ -10050,44 +10136,36 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" ht="209.25" customHeight="1">
+    <row r="61" spans="1:28" ht="171.6">
       <c r="A61" s="1"/>
       <c r="B61" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>405</v>
+        <v>231</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>423</v>
-      </c>
-      <c r="H61" s="16" t="s">
-        <v>432</v>
+        <v>140</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="I61" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J61" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="K61" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="L61" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="M61" s="21" t="s">
-        <v>415</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J61" s="13"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="14"/>
       <c r="N61" s="14"/>
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
@@ -10096,37 +10174,52 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
-    </row>
-    <row r="62" spans="1:28" ht="187.2">
+      <c r="V61" s="2"/>
+      <c r="W61" s="2"/>
+      <c r="X61" s="2"/>
+      <c r="Y61" s="2"/>
+      <c r="Z61" s="2"/>
+      <c r="AA61" s="2"/>
+      <c r="AB61" s="2"/>
+    </row>
+    <row r="62" spans="1:28" ht="209.25" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="13" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="H62" s="13" t="s">
-        <v>105</v>
+        <v>408</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>417</v>
       </c>
       <c r="I62" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J62" s="13"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-      <c r="M62" s="14"/>
+        <v>104</v>
+      </c>
+      <c r="J62" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="K62" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="L62" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="M62" s="21" t="s">
+        <v>400</v>
+      </c>
       <c r="N62" s="14"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -10135,33 +10228,32 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
-      <c r="V62" s="2"/>
-    </row>
-    <row r="63" spans="1:28" ht="327.60000000000002">
+    </row>
+    <row r="63" spans="1:28" ht="187.2">
       <c r="A63" s="1"/>
       <c r="B63" s="13" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I63" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J63" s="13"/>
       <c r="K63" s="18"/>
@@ -10177,31 +10269,31 @@
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="343.2">
+    <row r="64" spans="1:28" ht="327.60000000000002">
       <c r="A64" s="1"/>
       <c r="B64" s="13" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>248</v>
+        <v>365</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>404</v>
+        <v>369</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I64" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J64" s="13"/>
       <c r="K64" s="18"/>
@@ -10217,31 +10309,31 @@
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
     </row>
-    <row r="65" spans="1:22" ht="187.2">
+    <row r="65" spans="1:22" ht="343.2">
       <c r="A65" s="1"/>
       <c r="B65" s="13" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>244</v>
+        <v>389</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I65" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J65" s="13"/>
       <c r="K65" s="18"/>
@@ -10257,31 +10349,31 @@
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
     </row>
-    <row r="66" spans="1:22" ht="202.8">
+    <row r="66" spans="1:22" ht="187.2">
       <c r="A66" s="1"/>
       <c r="B66" s="13" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>385</v>
+        <v>233</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I66" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J66" s="13"/>
       <c r="K66" s="18"/>
@@ -10297,31 +10389,31 @@
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
     </row>
-    <row r="67" spans="1:22" ht="327.60000000000002">
+    <row r="67" spans="1:22" ht="202.8">
       <c r="A67" s="1"/>
       <c r="B67" s="13" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J67" s="13"/>
       <c r="K67" s="18"/>
@@ -10337,71 +10429,71 @@
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
     </row>
-    <row r="68" spans="1:22" ht="343.2">
+    <row r="68" spans="1:22" ht="327.60000000000002">
       <c r="A68" s="1"/>
       <c r="B68" s="13" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J68" s="13"/>
       <c r="K68" s="18"/>
       <c r="L68" s="18"/>
       <c r="M68" s="14"/>
       <c r="N68" s="14"/>
-      <c r="O68" s="11"/>
-      <c r="P68" s="11"/>
-      <c r="Q68" s="11"/>
-      <c r="R68" s="11"/>
-      <c r="S68" s="11"/>
-      <c r="T68" s="11"/>
-      <c r="U68" s="11"/>
-      <c r="V68" s="11"/>
-    </row>
-    <row r="69" spans="1:22" ht="156">
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="V68" s="2"/>
+    </row>
+    <row r="69" spans="1:22" ht="343.2">
       <c r="A69" s="1"/>
       <c r="B69" s="13" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J69" s="13"/>
       <c r="K69" s="18"/>
@@ -10417,29 +10509,31 @@
       <c r="U69" s="11"/>
       <c r="V69" s="11"/>
     </row>
-    <row r="70" spans="1:22" ht="140.4">
+    <row r="70" spans="1:22" ht="156">
       <c r="A70" s="1"/>
       <c r="B70" s="13" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="F70" s="24"/>
+        <v>373</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>179</v>
+      </c>
       <c r="G70" s="24" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J70" s="13"/>
       <c r="K70" s="18"/>
@@ -10453,71 +10547,70 @@
       <c r="S70" s="11"/>
       <c r="T70" s="11"/>
       <c r="U70" s="11"/>
-    </row>
-    <row r="71" spans="1:22" ht="173.4" customHeight="1">
+      <c r="V70" s="11"/>
+    </row>
+    <row r="71" spans="1:22" ht="140.4">
       <c r="A71" s="1"/>
       <c r="B71" s="13" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>390</v>
-      </c>
-      <c r="D71" s="26" t="s">
-        <v>202</v>
+        <v>240</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>189</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>389</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>203</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="F71" s="24"/>
       <c r="G71" s="24" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J71" s="13"/>
       <c r="K71" s="18"/>
       <c r="L71" s="18"/>
       <c r="M71" s="14"/>
       <c r="N71" s="14"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="2"/>
-      <c r="Q71" s="2"/>
-      <c r="R71" s="2"/>
-      <c r="S71" s="2"/>
-      <c r="T71" s="2"/>
-      <c r="U71" s="2"/>
-    </row>
-    <row r="72" spans="1:22" ht="171.6">
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
+      <c r="T71" s="11"/>
+      <c r="U71" s="11"/>
+    </row>
+    <row r="72" spans="1:22" ht="173.4" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="13" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>391</v>
-      </c>
-      <c r="D72" s="16" t="s">
-        <v>205</v>
+        <v>375</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>191</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J72" s="13"/>
       <c r="K72" s="18"/>
@@ -10535,28 +10628,28 @@
     <row r="73" spans="1:22" ht="171.6">
       <c r="A73" s="1"/>
       <c r="B73" s="13" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J73" s="13"/>
       <c r="K73" s="18"/>
@@ -10571,29 +10664,31 @@
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
     </row>
-    <row r="74" spans="1:22" ht="124.8">
+    <row r="74" spans="1:22" ht="171.6">
       <c r="A74" s="1"/>
       <c r="B74" s="13" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>408</v>
-      </c>
-      <c r="F74" s="24"/>
+        <v>379</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>192</v>
+      </c>
       <c r="G74" s="24" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J74" s="13"/>
       <c r="K74" s="18"/>
@@ -10611,28 +10706,26 @@
     <row r="75" spans="1:22" ht="124.8">
       <c r="A75" s="1"/>
       <c r="B75" s="13" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>411</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>412</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="F75" s="24"/>
       <c r="G75" s="24" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J75" s="13"/>
       <c r="K75" s="18"/>
@@ -10650,28 +10743,28 @@
     <row r="76" spans="1:22" ht="124.8">
       <c r="A76" s="1"/>
       <c r="B76" s="13" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="C76" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="F76" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="D76" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>203</v>
-      </c>
       <c r="G76" s="24" t="s">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J76" s="13"/>
       <c r="K76" s="18"/>
@@ -10689,28 +10782,28 @@
     <row r="77" spans="1:22" ht="124.8">
       <c r="A77" s="1"/>
       <c r="B77" s="13" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>413</v>
+        <v>382</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>118</v>
+        <v>200</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J77" s="13"/>
       <c r="K77" s="18"/>
@@ -10725,21 +10818,44 @@
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
     </row>
-    <row r="78" spans="1:22" ht="17.399999999999999">
+    <row r="78" spans="1:22" ht="124.8">
       <c r="A78" s="1"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
+      <c r="B78" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="C78" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G78" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I78" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J78" s="13"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="14"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="2"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="2"/>
+      <c r="S78" s="2"/>
+      <c r="T78" s="2"/>
+      <c r="U78" s="2"/>
     </row>
     <row r="79" spans="1:22" ht="17.399999999999999">
       <c r="A79" s="1"/>
@@ -11095,15 +11211,15 @@
     </row>
     <row r="101" spans="1:14" ht="17.399999999999999">
       <c r="A101" s="1"/>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="12"/>
-      <c r="I101" s="12"/>
-      <c r="J101" s="12"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
@@ -16976,26 +17092,10 @@
       <c r="H468" s="12"/>
       <c r="I468" s="12"/>
       <c r="J468" s="12"/>
-      <c r="K468" s="12"/>
-      <c r="L468" s="12"/>
-      <c r="M468" s="12"/>
-      <c r="N468" s="12"/>
-      <c r="O468" s="2"/>
-      <c r="P468" s="2"/>
-      <c r="Q468" s="2"/>
-      <c r="R468" s="2"/>
-      <c r="S468" s="2"/>
-      <c r="T468" s="2"/>
-      <c r="U468" s="2"/>
-      <c r="V468" s="2"/>
-      <c r="W468" s="2"/>
-      <c r="X468" s="2"/>
-      <c r="Y468" s="2"/>
-      <c r="Z468" s="2"/>
-      <c r="AA468" s="2"/>
-      <c r="AB468" s="2"/>
-      <c r="AC468" s="2"/>
-      <c r="AD468" s="2"/>
+      <c r="K468" s="2"/>
+      <c r="L468" s="2"/>
+      <c r="M468" s="2"/>
+      <c r="N468" s="2"/>
     </row>
     <row r="469" spans="1:30" ht="17.399999999999999">
       <c r="A469" s="1"/>
@@ -35335,6 +35435,19 @@
     </row>
     <row r="1042" spans="1:30" ht="17.399999999999999">
       <c r="A1042" s="1"/>
+      <c r="B1042" s="12"/>
+      <c r="C1042" s="12"/>
+      <c r="D1042" s="12"/>
+      <c r="E1042" s="12"/>
+      <c r="F1042" s="12"/>
+      <c r="G1042" s="12"/>
+      <c r="H1042" s="12"/>
+      <c r="I1042" s="12"/>
+      <c r="J1042" s="12"/>
+      <c r="K1042" s="12"/>
+      <c r="L1042" s="12"/>
+      <c r="M1042" s="12"/>
+      <c r="N1042" s="12"/>
       <c r="O1042" s="2"/>
       <c r="P1042" s="2"/>
       <c r="Q1042" s="2"/>
@@ -35352,8 +35465,27 @@
       <c r="AC1042" s="2"/>
       <c r="AD1042" s="2"/>
     </row>
+    <row r="1043" spans="1:30" ht="17.399999999999999">
+      <c r="A1043" s="1"/>
+      <c r="O1043" s="2"/>
+      <c r="P1043" s="2"/>
+      <c r="Q1043" s="2"/>
+      <c r="R1043" s="2"/>
+      <c r="S1043" s="2"/>
+      <c r="T1043" s="2"/>
+      <c r="U1043" s="2"/>
+      <c r="V1043" s="2"/>
+      <c r="W1043" s="2"/>
+      <c r="X1043" s="2"/>
+      <c r="Y1043" s="2"/>
+      <c r="Z1043" s="2"/>
+      <c r="AA1043" s="2"/>
+      <c r="AB1043" s="2"/>
+      <c r="AC1043" s="2"/>
+      <c r="AD1043" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B6:N28" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B6:N29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:Z1"/>
   </mergeCells>
@@ -35362,33 +35494,33 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L7:L77" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L7:L78" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"High,Medium,Low,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K7:K77" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K7:K78" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Blocker,Critical,Normal,Minor,Trival,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I7:I77" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I7:I78" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" location="/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{D92FC3DB-9442-4F18-8807-658358E245A2}"/>
-    <hyperlink ref="M13" r:id="rId3" location="DiE3fyyyVaIX" xr:uid="{2969F7C2-2C78-4EEE-83F8-DABC1323DCCC}"/>
-    <hyperlink ref="M14" r:id="rId4" location="KcJQSykpi0tN" xr:uid="{5E2256D7-17C1-4F51-9F97-88A58D2E1DA1}"/>
-    <hyperlink ref="M15" r:id="rId5" location="KcJQSykpi0tN" xr:uid="{99A4AB70-748F-45DE-B2E5-7DE382BA8178}"/>
-    <hyperlink ref="M16" r:id="rId6" location="KcJQSykpi0tN" xr:uid="{6F03D5C9-556F-46DD-B6D1-0F272B3D6BF4}"/>
-    <hyperlink ref="M17" r:id="rId7" location="KcJQSykpi0tN" xr:uid="{00B5DA23-082C-443C-90D6-73DEDA599F9C}"/>
-    <hyperlink ref="M20" r:id="rId8" location="KcJQSykpi0tN" xr:uid="{A76C7DBF-ABB6-41F3-A8D3-E914EB209254}"/>
-    <hyperlink ref="M21" r:id="rId9" location="KcJQSykpi0tN" xr:uid="{71F6DF8D-2C9B-43AB-ADCD-91ADBF863371}"/>
-    <hyperlink ref="M22" r:id="rId10" location="KcJQSykpi0tN" xr:uid="{03F1DFC9-32A9-4A01-B940-BF7EA04FCAD9}"/>
-    <hyperlink ref="M30" r:id="rId11" location="KcJQSykpi0tN" xr:uid="{8D7B1E87-54BB-42E4-B024-137ED5A19435}"/>
-    <hyperlink ref="M38" r:id="rId12" location="KcJQSykpi0tN" xr:uid="{EBF83787-3DEA-4CCE-9FBE-68F9D7638EF4}"/>
-    <hyperlink ref="M43" r:id="rId13" location="KcJQSykpi0tN" xr:uid="{3D35E54F-6F8A-4B14-8B08-D9525C522EA4}"/>
-    <hyperlink ref="M50" r:id="rId14" location="TMSEMduzmyPo" xr:uid="{171A6AAA-1830-4344-811D-ADB5DE71A196}"/>
-    <hyperlink ref="M54" r:id="rId15" location="TMSEMduzmyPo" xr:uid="{BF4F89E9-3310-4041-AC5A-3F2245959731}"/>
-    <hyperlink ref="M61" r:id="rId16" location="TMSEMduzmyPo" xr:uid="{F67F564C-E21F-4908-8B79-8F6464F7CEB8}"/>
+    <hyperlink ref="M14" r:id="rId3" location="DiE3fyyyVaIX" xr:uid="{2969F7C2-2C78-4EEE-83F8-DABC1323DCCC}"/>
+    <hyperlink ref="M15" r:id="rId4" location="KcJQSykpi0tN" xr:uid="{5E2256D7-17C1-4F51-9F97-88A58D2E1DA1}"/>
+    <hyperlink ref="M16" r:id="rId5" location="KcJQSykpi0tN" xr:uid="{99A4AB70-748F-45DE-B2E5-7DE382BA8178}"/>
+    <hyperlink ref="M17" r:id="rId6" location="KcJQSykpi0tN" xr:uid="{6F03D5C9-556F-46DD-B6D1-0F272B3D6BF4}"/>
+    <hyperlink ref="M18" r:id="rId7" location="KcJQSykpi0tN" xr:uid="{00B5DA23-082C-443C-90D6-73DEDA599F9C}"/>
+    <hyperlink ref="M21" r:id="rId8" location="KcJQSykpi0tN" xr:uid="{A76C7DBF-ABB6-41F3-A8D3-E914EB209254}"/>
+    <hyperlink ref="M22" r:id="rId9" location="KcJQSykpi0tN" xr:uid="{71F6DF8D-2C9B-43AB-ADCD-91ADBF863371}"/>
+    <hyperlink ref="M23" r:id="rId10" location="KcJQSykpi0tN" xr:uid="{03F1DFC9-32A9-4A01-B940-BF7EA04FCAD9}"/>
+    <hyperlink ref="M31" r:id="rId11" location="KcJQSykpi0tN" xr:uid="{8D7B1E87-54BB-42E4-B024-137ED5A19435}"/>
+    <hyperlink ref="M39" r:id="rId12" location="KcJQSykpi0tN" xr:uid="{EBF83787-3DEA-4CCE-9FBE-68F9D7638EF4}"/>
+    <hyperlink ref="M44" r:id="rId13" location="KcJQSykpi0tN" xr:uid="{3D35E54F-6F8A-4B14-8B08-D9525C522EA4}"/>
+    <hyperlink ref="M51" r:id="rId14" location="TMSEMduzmyPo" xr:uid="{171A6AAA-1830-4344-811D-ADB5DE71A196}"/>
+    <hyperlink ref="M55" r:id="rId15" location="TMSEMduzmyPo" xr:uid="{BF4F89E9-3310-4041-AC5A-3F2245959731}"/>
+    <hyperlink ref="M62" r:id="rId16" location="TMSEMduzmyPo" xr:uid="{F67F564C-E21F-4908-8B79-8F6464F7CEB8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>